<commit_message>
Graphs edited for Axis names
</commit_message>
<xml_diff>
--- a/Project1Graph.xlsx
+++ b/Project1Graph.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/honya/Documents/Computer Networks/Project 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74D28FD-2FDE-41C4-9EA6-953E06D9329F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="460" windowWidth="15420" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="13380" yWindow="465" windowWidth="15420" windowHeight="17535" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Option 1" sheetId="1" r:id="rId1"/>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -115,12 +116,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -159,7 +163,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -196,10 +199,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0573006889763779"/>
-          <c:y val="0.08416015625"/>
-          <c:w val="0.927074311023622"/>
-          <c:h val="0.775647607037401"/>
+          <c:x val="5.7300688976377898E-2"/>
+          <c:y val="8.4160156250000007E-2"/>
+          <c:w val="0.92707431102362203"/>
+          <c:h val="0.77564760703740099"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -263,7 +266,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -289,52 +291,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55.0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65.0</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -346,16 +348,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>10.85</c:v>
@@ -364,13 +366,13 @@
                   <c:v>13.48</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>17.1333333333333</c:v>
+                  <c:v>17.133333333333301</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.775</c:v>
+                  <c:v>21.774999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
                   <c:v>26.6444444444444</c:v>
@@ -382,13 +384,13 @@
                   <c:v>30.290909090909</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00">
-                  <c:v>40.4666666666666</c:v>
+                  <c:v>40.466666666666598</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00">
-                  <c:v>58.4923076923076</c:v>
+                  <c:v>58.492307692307598</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00">
-                  <c:v>62.2142857142857</c:v>
+                  <c:v>62.214285714285701</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>67.36</c:v>
@@ -397,6 +399,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7C7C-4FA2-BC39-74DD990F805E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -453,7 +460,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -479,52 +485,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55.0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65.0</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -536,16 +542,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>10.85</c:v>
@@ -554,13 +560,13 @@
                   <c:v>13.48</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>17.1333333333333</c:v>
+                  <c:v>17.133333333333301</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.775</c:v>
+                  <c:v>21.774999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
                   <c:v>26.6444444444444</c:v>
@@ -572,13 +578,13 @@
                   <c:v>30.290909090909</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00">
-                  <c:v>40.4666666666666</c:v>
+                  <c:v>40.466666666666598</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00">
-                  <c:v>58.4923076923076</c:v>
+                  <c:v>58.492307692307598</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00">
-                  <c:v>62.2142857142857</c:v>
+                  <c:v>62.214285714285701</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>67.36</c:v>
@@ -587,6 +593,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7C7C-4FA2-BC39-74DD990F805E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="r"/>
@@ -634,7 +645,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -755,7 +765,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -785,6 +794,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -833,7 +843,6 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -901,7 +910,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -935,12 +944,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Date and Time</a:t>
+              <a:t>Client Count vs Mean response Time (Light Load, Date&amp;Time)</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -977,10 +985,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0573006889763779"/>
-          <c:y val="0.08416015625"/>
-          <c:w val="0.927074311023622"/>
-          <c:h val="0.775647607037401"/>
+          <c:x val="5.7300688976377898E-2"/>
+          <c:y val="8.4160156250000007E-2"/>
+          <c:w val="0.92707431102362203"/>
+          <c:h val="0.77564760703740099"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1044,7 +1052,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1070,52 +1077,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55.0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65.0</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,16 +1134,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>10.85</c:v>
@@ -1145,13 +1152,13 @@
                   <c:v>13.48</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>17.1333333333333</c:v>
+                  <c:v>17.133333333333301</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.775</c:v>
+                  <c:v>21.774999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
                   <c:v>26.6444444444444</c:v>
@@ -1163,13 +1170,13 @@
                   <c:v>30.290909090909</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00">
-                  <c:v>40.4666666666666</c:v>
+                  <c:v>40.466666666666598</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00">
-                  <c:v>58.4923076923076</c:v>
+                  <c:v>58.492307692307598</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00">
-                  <c:v>62.2142857142857</c:v>
+                  <c:v>62.214285714285701</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>67.36</c:v>
@@ -1178,6 +1185,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-28A8-4BDB-88D8-680714DF40A1}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1237,7 +1249,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1263,52 +1274,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55.0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65.0</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1320,16 +1331,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>10.85</c:v>
@@ -1338,13 +1349,13 @@
                   <c:v>13.48</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>17.1333333333333</c:v>
+                  <c:v>17.133333333333301</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.775</c:v>
+                  <c:v>21.774999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
                   <c:v>26.6444444444444</c:v>
@@ -1356,13 +1367,13 @@
                   <c:v>30.290909090909</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00">
-                  <c:v>40.4666666666666</c:v>
+                  <c:v>40.466666666666598</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00">
-                  <c:v>58.4923076923076</c:v>
+                  <c:v>58.492307692307598</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00">
-                  <c:v>62.2142857142857</c:v>
+                  <c:v>62.214285714285701</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>67.36</c:v>
@@ -1371,6 +1382,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-28A8-4BDB-88D8-680714DF40A1}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="r"/>
@@ -1418,7 +1434,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1534,12 +1549,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of Clients</a:t>
+                  <a:t>Mean Response Time (in milliseconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1569,6 +1583,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1617,7 +1632,6 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1685,7 +1699,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1719,12 +1733,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Netstat</a:t>
+              <a:t>Client Count vs Mean Response Time (Heavy</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Load, NetStat)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1815,7 +1833,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1841,52 +1858,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55.0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65.0</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1898,46 +1915,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.4</c:v>
+                  <c:v>16.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24.4</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00">
-                  <c:v>30.2666666666666</c:v>
+                  <c:v>30.266666666666602</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>50.76</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>60.5666666666666</c:v>
+                  <c:v>60.566666666666599</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00">
-                  <c:v>71.9714285714285</c:v>
+                  <c:v>71.971428571428504</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>83.35</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
-                  <c:v>96.28888888888881</c:v>
+                  <c:v>96.288888888888806</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>114.44</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>123.0</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00">
                   <c:v>124.266666666666</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00">
-                  <c:v>132.846153846153</c:v>
+                  <c:v>132.84615384615299</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>150.5</c:v>
@@ -1949,6 +1966,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F6F4-4036-9D21-691D8D92EF74}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2008,7 +2030,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2034,52 +2055,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55.0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65.0</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2091,46 +2112,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.4</c:v>
+                  <c:v>16.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24.4</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00">
-                  <c:v>30.2666666666666</c:v>
+                  <c:v>30.266666666666602</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>50.76</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>60.5666666666666</c:v>
+                  <c:v>60.566666666666599</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00">
-                  <c:v>71.9714285714285</c:v>
+                  <c:v>71.971428571428504</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>83.35</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
-                  <c:v>96.28888888888881</c:v>
+                  <c:v>96.288888888888806</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>114.44</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>123.0</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00">
                   <c:v>124.266666666666</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00">
-                  <c:v>132.846153846153</c:v>
+                  <c:v>132.84615384615299</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>150.5</c:v>
@@ -2142,6 +2163,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F6F4-4036-9D21-691D8D92EF74}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="b"/>
@@ -2163,6 +2189,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Clients</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2228,6 +2309,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mean Response Time (in milliseconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2276,7 +2413,6 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4028,7 +4164,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4058,7 +4200,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4093,7 +4241,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4373,20 +4527,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4394,7 +4548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4402,7 +4556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -4410,7 +4564,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -4418,7 +4572,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -4426,7 +4580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -4434,7 +4588,7 @@
         <v>10.85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -4442,7 +4596,7 @@
         <v>13.48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -4450,7 +4604,7 @@
         <v>17.133333333333301</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>35</v>
       </c>
@@ -4458,7 +4612,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -4466,7 +4620,7 @@
         <v>21.774999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>45</v>
       </c>
@@ -4474,7 +4628,7 @@
         <v>26.6444444444444</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
@@ -4482,7 +4636,7 @@
         <v>28.04</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>55</v>
       </c>
@@ -4490,7 +4644,7 @@
         <v>30.290909090909</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>60</v>
       </c>
@@ -4498,7 +4652,7 @@
         <v>40.466666666666598</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>65</v>
       </c>
@@ -4506,7 +4660,7 @@
         <v>58.492307692307598</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>70</v>
       </c>
@@ -4514,7 +4668,7 @@
         <v>62.214285714285701</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>75</v>
       </c>
@@ -4522,17 +4676,17 @@
         <v>67.36</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -4545,19 +4699,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4565,7 +4719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4573,7 +4727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -4581,7 +4735,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -4589,7 +4743,7 @@
         <v>24.4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -4597,7 +4751,7 @@
         <v>30.266666666666602</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -4605,7 +4759,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -4613,7 +4767,7 @@
         <v>50.76</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -4621,7 +4775,7 @@
         <v>60.566666666666599</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>35</v>
       </c>
@@ -4629,7 +4783,7 @@
         <v>71.971428571428504</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -4637,7 +4791,7 @@
         <v>83.35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>45</v>
       </c>
@@ -4645,7 +4799,7 @@
         <v>96.288888888888806</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
@@ -4653,7 +4807,7 @@
         <v>114.44</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>55</v>
       </c>
@@ -4661,7 +4815,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>60</v>
       </c>
@@ -4669,7 +4823,7 @@
         <v>124.266666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>65</v>
       </c>
@@ -4677,7 +4831,7 @@
         <v>132.84615384615299</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>70</v>
       </c>
@@ -4685,7 +4839,7 @@
         <v>150.5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>75</v>
       </c>
@@ -4693,17 +4847,17 @@
         <v>177.52</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>2</v>
       </c>

</xml_diff>